<commit_message>
commit realizado em: 2025-07-26
</commit_message>
<xml_diff>
--- a/Metodologias.xlsx
+++ b/Metodologias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5093564b1391b0aa/Área de Trabalho/POSMARH/Materiais/APP-ÍNDICES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F3BDCFE-487E-4270-99A4-3DCC99A52718}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0EA2B69-1B23-4297-B9B6-B30D7E4FE7E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="112">
   <si>
     <t>Niño 1.2 (°C)</t>
   </si>
@@ -112,9 +112,6 @@
     <t xml:space="preserve">SSTRG2 (°C) </t>
   </si>
   <si>
-    <t>SST anomalies are computed for the cyclogenetic region located between Uruguay and the extreme south of Brazil (RG2): 40ºS-30ºS and 57º-47ºW</t>
-  </si>
-  <si>
     <t>The Indian Ocean Subtropical Dipole (IOSD) index is defined as the difference between SST anomalies in the western (55°E–65°E, 27°S–37°S) and eastern (90°E–100°E, 18°S–28°S) centers of the dipole.</t>
   </si>
   <si>
@@ -647,6 +644,72 @@
   </si>
   <si>
     <t>NIN04</t>
+  </si>
+  <si>
+    <t>Antarctic Oscillation</t>
+  </si>
+  <si>
+    <t>Arctic Oscillation</t>
+  </si>
+  <si>
+    <t>Name_Index</t>
+  </si>
+  <si>
+    <t>Indian Ocean Dipole</t>
+  </si>
+  <si>
+    <t>Indian Ocean Subtropical Dipole</t>
+  </si>
+  <si>
+    <t>North Atlantic Oscillation</t>
+  </si>
+  <si>
+    <t>Niño 1.2</t>
+  </si>
+  <si>
+    <t>Niño 3</t>
+  </si>
+  <si>
+    <t>Niño 3.4</t>
+  </si>
+  <si>
+    <t>Niño 4</t>
+  </si>
+  <si>
+    <t>Pacific North America</t>
+  </si>
+  <si>
+    <t>Pacific South American</t>
+  </si>
+  <si>
+    <t>Real-time Multivariate MJO</t>
+  </si>
+  <si>
+    <t>South Atlantic Dipole</t>
+  </si>
+  <si>
+    <t>South Atlantic Ocean Dipole</t>
+  </si>
+  <si>
+    <t>South Atlantic Subtropical Anticyclone Index</t>
+  </si>
+  <si>
+    <t>South Atlantic Subtropical Dipole</t>
+  </si>
+  <si>
+    <t>Southern Oscillation Index</t>
+  </si>
+  <si>
+    <t>SST anomalies</t>
+  </si>
+  <si>
+    <t>Tropical South Atlantic</t>
+  </si>
+  <si>
+    <t>Tropical North Atlantic</t>
+  </si>
+  <si>
+    <t>SST anomalies are computed for the cyclogenetic region located between Uruguay and the extreme south of Brazil (RG2): 40ºS-30ºS and 57º-47ºW.</t>
   </si>
 </sst>
 </file>
@@ -706,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -719,11 +782,120 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -783,100 +955,15 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -889,18 +976,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}" name="Tabela1" displayName="Tabela1" ref="A1:F22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F22" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}" name="Tabela1" displayName="Tabela1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G22" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G22">
     <sortCondition ref="A1:A22"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3EAE4E6C-889B-48C6-AAF8-DB3BD35DACB1}" name="Index" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{DA40A391-2AFF-4B89-BD7E-84EF0E25192D}" name="Unit" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{A03739CF-C01D-4871-9EC2-D824327EC32F}" name="Index_Unit" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{D87511CF-DDA9-43F3-BBE2-BA25C96A6C7B}" name="Methodology" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{942D9726-6821-405A-99AE-8614615DCEED}" name="Access" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{66C0787D-ABB6-4F4B-8E13-AEE7386C0EB5}" name="Reference" dataDxfId="2"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{3EAE4E6C-889B-48C6-AAF8-DB3BD35DACB1}" name="Index" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DA40A391-2AFF-4B89-BD7E-84EF0E25192D}" name="Unit" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{A03739CF-C01D-4871-9EC2-D824327EC32F}" name="Index_Unit" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{82A22D2B-A456-475F-8BF8-973032739F53}" name="Name_Index" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D87511CF-DDA9-43F3-BBE2-BA25C96A6C7B}" name="Methodology" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{942D9726-6821-405A-99AE-8614615DCEED}" name="Access" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{66C0787D-ABB6-4F4B-8E13-AEE7386C0EB5}" name="Reference" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1169,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1180,494 +1268,567 @@
     <col min="1" max="1" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="94.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="4" max="4" width="43.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="94.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="46.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="B7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" xr:uid="{AC8C0971-FBAE-4BE0-AAA7-CBC1800B34DC}"/>
-    <hyperlink ref="E9" r:id="rId2" xr:uid="{245EB88A-FE7C-43E9-9638-22C6D9E40350}"/>
-    <hyperlink ref="E10" r:id="rId3" xr:uid="{B9DFECB3-E987-4FF4-9697-4725A45D27B6}"/>
-    <hyperlink ref="E7" r:id="rId4" xr:uid="{ECA62230-534D-4F97-8A6C-63B4E3B96DD4}"/>
-    <hyperlink ref="E19" r:id="rId5" location="SOICALC" display="https://www.cpc.ncep.noaa.gov/data/indices/Readme.index.shtml - SOICALC" xr:uid="{B1D8E77E-2473-482E-BCB2-61498215E874}"/>
-    <hyperlink ref="E22" r:id="rId6" xr:uid="{5C08678B-DCCB-4DB1-A396-05DF1D44A233}"/>
-    <hyperlink ref="E21" r:id="rId7" xr:uid="{414AFD97-2A29-45BD-91E9-7FE87FE43269}"/>
-    <hyperlink ref="E16" r:id="rId8" xr:uid="{7D930AD2-BB31-4516-9F29-81BF351BCDBC}"/>
-    <hyperlink ref="E18" r:id="rId9" xr:uid="{C8785809-3965-4F85-A971-059C01941277}"/>
-    <hyperlink ref="E17" r:id="rId10" xr:uid="{9228F806-3134-4A5D-8563-43A5E0031DB2}"/>
-    <hyperlink ref="E20" r:id="rId11" xr:uid="{A3FDF396-DAE3-42F7-87E6-4CAB4933AD41}"/>
-    <hyperlink ref="E5" r:id="rId12" xr:uid="{14120442-89A1-4A75-8BE4-5C765C37105E}"/>
-    <hyperlink ref="E4" r:id="rId13" xr:uid="{F20588DE-6804-4152-A357-5A75E889272F}"/>
-    <hyperlink ref="E3" r:id="rId14" xr:uid="{0785A3D1-3333-498E-AD13-B78338D847DD}"/>
-    <hyperlink ref="E2" r:id="rId15" xr:uid="{1F753BAD-2D85-41DD-8F6B-4B8BF4631DCF}"/>
-    <hyperlink ref="E11" r:id="rId16" xr:uid="{4C36545A-5849-4991-96E7-96B1A53C7F73}"/>
-    <hyperlink ref="E12" r:id="rId17" xr:uid="{46C9D95C-9794-402B-81E1-6EB4A8F03EFD}"/>
-    <hyperlink ref="E13" r:id="rId18" display="https://meteorologia.unifei.edu.br/teleconexoes/indice?id=psa2" xr:uid="{644E1F58-4995-4E43-A95E-032B9E58B994}"/>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{AC8C0971-FBAE-4BE0-AAA7-CBC1800B34DC}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{245EB88A-FE7C-43E9-9638-22C6D9E40350}"/>
+    <hyperlink ref="F10" r:id="rId3" xr:uid="{B9DFECB3-E987-4FF4-9697-4725A45D27B6}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{ECA62230-534D-4F97-8A6C-63B4E3B96DD4}"/>
+    <hyperlink ref="F19" r:id="rId5" location="SOICALC" display="https://www.cpc.ncep.noaa.gov/data/indices/Readme.index.shtml - SOICALC" xr:uid="{B1D8E77E-2473-482E-BCB2-61498215E874}"/>
+    <hyperlink ref="F22" r:id="rId6" xr:uid="{5C08678B-DCCB-4DB1-A396-05DF1D44A233}"/>
+    <hyperlink ref="F21" r:id="rId7" xr:uid="{414AFD97-2A29-45BD-91E9-7FE87FE43269}"/>
+    <hyperlink ref="F16" r:id="rId8" xr:uid="{7D930AD2-BB31-4516-9F29-81BF351BCDBC}"/>
+    <hyperlink ref="F18" r:id="rId9" xr:uid="{C8785809-3965-4F85-A971-059C01941277}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{9228F806-3134-4A5D-8563-43A5E0031DB2}"/>
+    <hyperlink ref="F20" r:id="rId11" xr:uid="{A3FDF396-DAE3-42F7-87E6-4CAB4933AD41}"/>
+    <hyperlink ref="F5" r:id="rId12" xr:uid="{14120442-89A1-4A75-8BE4-5C765C37105E}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{F20588DE-6804-4152-A357-5A75E889272F}"/>
+    <hyperlink ref="F3" r:id="rId14" xr:uid="{0785A3D1-3333-498E-AD13-B78338D847DD}"/>
+    <hyperlink ref="F2" r:id="rId15" xr:uid="{1F753BAD-2D85-41DD-8F6B-4B8BF4631DCF}"/>
+    <hyperlink ref="F11" r:id="rId16" xr:uid="{4C36545A-5849-4991-96E7-96B1A53C7F73}"/>
+    <hyperlink ref="F12" r:id="rId17" xr:uid="{46C9D95C-9794-402B-81E1-6EB4A8F03EFD}"/>
+    <hyperlink ref="F13" r:id="rId18" display="https://meteorologia.unifei.edu.br/teleconexoes/indice?id=psa2" xr:uid="{644E1F58-4995-4E43-A95E-032B9E58B994}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
commit realizado em: 2025-07-27
</commit_message>
<xml_diff>
--- a/Metodologias.xlsx
+++ b/Metodologias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5093564b1391b0aa/Área de Trabalho/POSMARH/Materiais/APP-ÍNDICES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0EA2B69-1B23-4297-B9B6-B30D7E4FE7E4}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BE2B098-026A-4C70-8F6B-E5A34365E451}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,85 +631,85 @@
     <t>Index_Unit</t>
   </si>
   <si>
+    <t>Antarctic Oscillation</t>
+  </si>
+  <si>
+    <t>Arctic Oscillation</t>
+  </si>
+  <si>
+    <t>Name_Index</t>
+  </si>
+  <si>
+    <t>Indian Ocean Dipole</t>
+  </si>
+  <si>
+    <t>Indian Ocean Subtropical Dipole</t>
+  </si>
+  <si>
+    <t>North Atlantic Oscillation</t>
+  </si>
+  <si>
+    <t>Niño 1.2</t>
+  </si>
+  <si>
+    <t>Niño 3</t>
+  </si>
+  <si>
+    <t>Niño 3.4</t>
+  </si>
+  <si>
+    <t>Niño 4</t>
+  </si>
+  <si>
+    <t>Pacific North America</t>
+  </si>
+  <si>
+    <t>Pacific South American</t>
+  </si>
+  <si>
+    <t>Real-time Multivariate MJO</t>
+  </si>
+  <si>
+    <t>South Atlantic Dipole</t>
+  </si>
+  <si>
+    <t>South Atlantic Ocean Dipole</t>
+  </si>
+  <si>
+    <t>South Atlantic Subtropical Anticyclone Index</t>
+  </si>
+  <si>
+    <t>South Atlantic Subtropical Dipole</t>
+  </si>
+  <si>
+    <t>Southern Oscillation Index</t>
+  </si>
+  <si>
+    <t>SST anomalies</t>
+  </si>
+  <si>
+    <t>Tropical South Atlantic</t>
+  </si>
+  <si>
+    <t>Tropical North Atlantic</t>
+  </si>
+  <si>
+    <t>SST anomalies are computed for the cyclogenetic region located between Uruguay and the extreme south of Brazil (RG2): 40ºS-30ºS and 57º-47ºW.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIN12 </t>
+  </si>
+  <si>
+    <t>NIN34</t>
+  </si>
+  <si>
+    <t>NIN04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIN03 </t>
+  </si>
+  <si>
     <t>DMI/IOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NIN12 </t>
-  </si>
-  <si>
-    <t>NIN34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NIN03 </t>
-  </si>
-  <si>
-    <t>NIN04</t>
-  </si>
-  <si>
-    <t>Antarctic Oscillation</t>
-  </si>
-  <si>
-    <t>Arctic Oscillation</t>
-  </si>
-  <si>
-    <t>Name_Index</t>
-  </si>
-  <si>
-    <t>Indian Ocean Dipole</t>
-  </si>
-  <si>
-    <t>Indian Ocean Subtropical Dipole</t>
-  </si>
-  <si>
-    <t>North Atlantic Oscillation</t>
-  </si>
-  <si>
-    <t>Niño 1.2</t>
-  </si>
-  <si>
-    <t>Niño 3</t>
-  </si>
-  <si>
-    <t>Niño 3.4</t>
-  </si>
-  <si>
-    <t>Niño 4</t>
-  </si>
-  <si>
-    <t>Pacific North America</t>
-  </si>
-  <si>
-    <t>Pacific South American</t>
-  </si>
-  <si>
-    <t>Real-time Multivariate MJO</t>
-  </si>
-  <si>
-    <t>South Atlantic Dipole</t>
-  </si>
-  <si>
-    <t>South Atlantic Ocean Dipole</t>
-  </si>
-  <si>
-    <t>South Atlantic Subtropical Anticyclone Index</t>
-  </si>
-  <si>
-    <t>South Atlantic Subtropical Dipole</t>
-  </si>
-  <si>
-    <t>Southern Oscillation Index</t>
-  </si>
-  <si>
-    <t>SST anomalies</t>
-  </si>
-  <si>
-    <t>Tropical South Atlantic</t>
-  </si>
-  <si>
-    <t>Tropical North Atlantic</t>
-  </si>
-  <si>
-    <t>SST anomalies are computed for the cyclogenetic region located between Uruguay and the extreme south of Brazil (RG2): 40ºS-30ºS and 57º-47ºW.</t>
   </si>
 </sst>
 </file>
@@ -1259,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1286,7 @@
         <v>84</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -1310,7 +1310,7 @@
         <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>48</v>
@@ -1334,7 +1334,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>35</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="4" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>80</v>
@@ -1358,7 +1358,7 @@
         <v>62</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>31</v>
@@ -1382,7 +1382,7 @@
         <v>61</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>28</v>
@@ -1406,7 +1406,7 @@
         <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>56</v>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="7" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>80</v>
@@ -1430,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>60</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="8" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>80</v>
@@ -1454,7 +1454,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>60</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="9" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>80</v>
@@ -1478,7 +1478,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>60</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="10" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>80</v>
@@ -1502,7 +1502,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>60</v>
@@ -1526,7 +1526,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>56</v>
@@ -1550,7 +1550,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>47</v>
@@ -1574,7 +1574,7 @@
         <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>46</v>
@@ -1598,7 +1598,7 @@
         <v>44</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>45</v>
@@ -1622,7 +1622,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>59</v>
@@ -1646,7 +1646,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>54</v>
@@ -1670,7 +1670,7 @@
         <v>23</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>24</v>
@@ -1694,7 +1694,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>54</v>
@@ -1718,7 +1718,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>10</v>
@@ -1742,10 +1742,10 @@
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>25</v>
@@ -1766,7 +1766,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>15</v>
@@ -1790,7 +1790,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
commit realizado em: 2025-07-28
</commit_message>
<xml_diff>
--- a/Metodologias.xlsx
+++ b/Metodologias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5093564b1391b0aa/Área de Trabalho/POSMARH/Materiais/APP-ÍNDICES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BE2B098-026A-4C70-8F6B-E5A34365E451}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46E1A81E-346E-4507-AD59-966E41551115}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="128">
   <si>
     <t>Niño 1.2 (°C)</t>
   </si>
@@ -710,6 +710,54 @@
   </si>
   <si>
     <t>DMI/IOD</t>
+  </si>
+  <si>
+    <t>AMO</t>
+  </si>
+  <si>
+    <t>AMO (°C)</t>
+  </si>
+  <si>
+    <t>Atlantic Multidecadal Oscillation</t>
+  </si>
+  <si>
+    <t>The timeseries are calculated from the Kaplan SST dataset which is updated monthly. It is basically an index of the N Atlantic temperatures. Time series are created; a smoothed version and an unsmoothed version. In addition, two files starting at 1948 are produced to be used in the Correlation webpages.</t>
+  </si>
+  <si>
+    <t>Enfield et al. (2001)</t>
+  </si>
+  <si>
+    <t>Three month running mean of NOAA ERSST.V5 SST anomalies in the Niño 3.4 region (5N-5S, 120-170W), based on changing base period which onsist of multiple centered 30-year base periods. These 30-year base periods will be used to calculate the anomalies for successive 5-year periods in the historical record.</t>
+  </si>
+  <si>
+    <t>Pacific Decadal Oscillation</t>
+  </si>
+  <si>
+    <t>Oceanic Niño Index</t>
+  </si>
+  <si>
+    <t>ONI</t>
+  </si>
+  <si>
+    <t>PDO</t>
+  </si>
+  <si>
+    <t>ONI (°C)</t>
+  </si>
+  <si>
+    <t>PDO (°C)</t>
+  </si>
+  <si>
+    <t>PDO is the leading PC of monthly SST anomalies in the North Pacific Ocean.</t>
+  </si>
+  <si>
+    <t>QBO</t>
+  </si>
+  <si>
+    <t>Quasi-Biennial Oscillation</t>
+  </si>
+  <si>
+    <t>Calculated at PSL (from the zonal average of the 30mb zonal wind at the equator as computed from the NCEP/NCAR Reanalysis).</t>
   </si>
 </sst>
 </file>
@@ -769,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -783,6 +831,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,12 +964,6 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -937,6 +982,12 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -976,19 +1027,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}" name="Tabela1" displayName="Tabela1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G22" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}" name="Tabela1" displayName="Tabela1" ref="A1:G26" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
+  <autoFilter ref="A1:G26" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3EAE4E6C-889B-48C6-AAF8-DB3BD35DACB1}" name="Index" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DA40A391-2AFF-4B89-BD7E-84EF0E25192D}" name="Unit" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{A03739CF-C01D-4871-9EC2-D824327EC32F}" name="Index_Unit" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{82A22D2B-A456-475F-8BF8-973032739F53}" name="Name_Index" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{D87511CF-DDA9-43F3-BBE2-BA25C96A6C7B}" name="Methodology" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{942D9726-6821-405A-99AE-8614615DCEED}" name="Access" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{66C0787D-ABB6-4F4B-8E13-AEE7386C0EB5}" name="Reference" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3EAE4E6C-889B-48C6-AAF8-DB3BD35DACB1}" name="Index" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{DA40A391-2AFF-4B89-BD7E-84EF0E25192D}" name="Unit" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{A03739CF-C01D-4871-9EC2-D824327EC32F}" name="Index_Unit" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{82A22D2B-A456-475F-8BF8-973032739F53}" name="Name_Index" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{D87511CF-DDA9-43F3-BBE2-BA25C96A6C7B}" name="Methodology" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{942D9726-6821-405A-99AE-8614615DCEED}" name="Access" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{66C0787D-ABB6-4F4B-8E13-AEE7386C0EB5}" name="Reference" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1257,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="D14" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1803,11 +1854,94 @@
       </c>
       <c r="H22" s="2"/>
     </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="6"/>
+    </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E29" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
commit realizado em: 2025-08-07
</commit_message>
<xml_diff>
--- a/Metodologias.xlsx
+++ b/Metodologias.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5093564b1391b0aa/Área de Trabalho/POSMARH/Materiais/APP-ÍNDICES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="212" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46E1A81E-346E-4507-AD59-966E41551115}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3BC2427-4E53-428A-BA3E-4F28C4E41EF9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="128">
   <si>
     <t>Niño 1.2 (°C)</t>
   </si>
@@ -964,6 +964,12 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -982,12 +988,6 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1027,19 +1027,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}" name="Tabela1" displayName="Tabela1" ref="A1:G26" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}" name="Tabela1" displayName="Tabela1" ref="A1:G26" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G26" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3EAE4E6C-889B-48C6-AAF8-DB3BD35DACB1}" name="Index" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{DA40A391-2AFF-4B89-BD7E-84EF0E25192D}" name="Unit" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{A03739CF-C01D-4871-9EC2-D824327EC32F}" name="Index_Unit" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{82A22D2B-A456-475F-8BF8-973032739F53}" name="Name_Index" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{D87511CF-DDA9-43F3-BBE2-BA25C96A6C7B}" name="Methodology" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{942D9726-6821-405A-99AE-8614615DCEED}" name="Access" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{66C0787D-ABB6-4F4B-8E13-AEE7386C0EB5}" name="Reference" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3EAE4E6C-889B-48C6-AAF8-DB3BD35DACB1}" name="Index" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DA40A391-2AFF-4B89-BD7E-84EF0E25192D}" name="Unit" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{A03739CF-C01D-4871-9EC2-D824327EC32F}" name="Index_Unit" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{82A22D2B-A456-475F-8BF8-973032739F53}" name="Name_Index" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D87511CF-DDA9-43F3-BBE2-BA25C96A6C7B}" name="Methodology" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{942D9726-6821-405A-99AE-8614615DCEED}" name="Access" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{66C0787D-ABB6-4F4B-8E13-AEE7386C0EB5}" name="Reference" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1896,6 +1896,9 @@
       <c r="F24" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="G24" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -1916,6 +1919,9 @@
       <c r="F25" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="G25" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1935,6 +1941,9 @@
       </c>
       <c r="F26" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
commit realizado em: 2025-08-14
</commit_message>
<xml_diff>
--- a/Metodologias.xlsx
+++ b/Metodologias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5093564b1391b0aa/Área de Trabalho/POSMARH/Materiais/APP-ÍNDICES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3BC2427-4E53-428A-BA3E-4F28C4E41EF9}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB8CA2ED-F749-4A72-9235-DE54F2559D6D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,9 +160,6 @@
     <t>PSA2 (dimensionless)</t>
   </si>
   <si>
-    <t>RMM (dimensionless)</t>
-  </si>
-  <si>
     <t>The Real-time Multivariate MJO (RMM) Index is used to monitor the Madden–Julian Oscillation (MJO). It is based on three daily variables from the equatorial belt (15°S–15°N): outgoing longwave radiation, zonal wind at 850 hPa and 200 hPa. Before computing the combined EOF, the annual cycle is removed from the data, and only the intraseasonal variability (frequencies between 20 and 100 days) is retained using a Lanczos filter. The principal components corresponding to the first two EOFs, referred to as RMM1 and RMM2, define the real-time MJO index.</t>
   </si>
   <si>
@@ -613,9 +610,6 @@
     <t xml:space="preserve">PSA2 </t>
   </si>
   <si>
-    <t xml:space="preserve">RMM </t>
-  </si>
-  <si>
     <t>(°C)</t>
   </si>
   <si>
@@ -758,6 +752,12 @@
   </si>
   <si>
     <t>Calculated at PSL (from the zonal average of the 30mb zonal wind at the equator as computed from the NCEP/NCAR Reanalysis).</t>
+  </si>
+  <si>
+    <t>MJO</t>
+  </si>
+  <si>
+    <t>MJO (dimensionless)</t>
   </si>
 </sst>
 </file>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1328,22 +1328,22 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
@@ -1352,40 +1352,40 @@
     </row>
     <row r="2" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>35</v>
@@ -1394,22 +1394,22 @@
         <v>36</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>31</v>
@@ -1424,16 +1424,16 @@
     </row>
     <row r="5" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>28</v>
@@ -1448,19 +1448,19 @@
     </row>
     <row r="6" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>40</v>
@@ -1472,19 +1472,19 @@
     </row>
     <row r="7" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
@@ -1496,19 +1496,19 @@
     </row>
     <row r="8" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>8</v>
@@ -1520,19 +1520,19 @@
     </row>
     <row r="9" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>8</v>
@@ -1544,19 +1544,19 @@
     </row>
     <row r="10" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>8</v>
@@ -1568,19 +1568,19 @@
     </row>
     <row r="11" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>39</v>
@@ -1592,115 +1592,115 @@
     </row>
     <row r="12" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="C14" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>19</v>
@@ -1712,16 +1712,16 @@
     </row>
     <row r="17" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>24</v>
@@ -1736,19 +1736,19 @@
     </row>
     <row r="18" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>19</v>
@@ -1760,16 +1760,16 @@
     </row>
     <row r="19" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>10</v>
@@ -1784,19 +1784,19 @@
     </row>
     <row r="20" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>25</v>
@@ -1808,16 +1808,16 @@
     </row>
     <row r="21" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>15</v>
@@ -1832,16 +1832,16 @@
     </row>
     <row r="22" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>15</v>
@@ -1856,42 +1856,42 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>6</v>
@@ -1902,19 +1902,19 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="D25" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>6</v>
@@ -1925,19 +1925,19 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
commit realizado em: 2026-01-02
</commit_message>
<xml_diff>
--- a/Metodologias.xlsx
+++ b/Metodologias.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5093564b1391b0aa/Área de Trabalho/POSMARH/Materiais/APP-ÍNDICES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB8CA2ED-F749-4A72-9235-DE54F2559D6D}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="8_{FC8637FF-0F44-4418-B80D-DD67B6FA12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3D86F31-7331-4F6B-824F-20519F4A0A7B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="131">
   <si>
     <t>Niño 1.2 (°C)</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Wheeler and Hendon (2004)</t>
   </si>
   <si>
-    <t>Nogueira et al. (2025)</t>
-  </si>
-  <si>
     <t>The South Atlantic Ocean Dipole (SAODI; Nnamchi and Anyadike, 2011) and the South Atlantic Subtropical Dipole (SASDI; Morioka et al., 2011) indices capture distinct aspects of South Atlantic Dipole variability (Nnamchi et al., 2017). The SAODI is defined as the difference between domain-averaged SST anomalies over the northeast pole (NEP; 10°E–20°W, 0°–15°S) and the southwest pole (SWP; 10°W–40°W, 25°–40°S). In contrast, the SASDI defines the NEP as 0°–20°W, 15°S–25°S, and the SWP as 10°W–30°W, 30°S–40°S. Originally, the SASDI was defined as the difference between the SWP and the NEP. Here, we inverted this definition to maintain consistency between both indices.</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t>Access</t>
   </si>
   <si>
-    <t xml:space="preserve">The South Atlantic Dipole (SAD) is computed based on SST anomalies standardized using the standard deviation for the period 1991–2020 in the South Atlantic Ocean. Based on the previous approaches proposed by Morioka and Nnamchi, Empirical Orthogonal Function (EOF) analysis is applied for each calendar month, and the EOF corresponding to the SAD pattern is then selected. </t>
-  </si>
-  <si>
     <r>
       <t>SST anomalies are computed for each region representative of the different Niños: Niño 1.2: 90</t>
     </r>
@@ -758,6 +752,21 @@
   </si>
   <si>
     <t>MJO (dimensionless)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The South Atlantic Dipole (SAD)  is characterized by a northeast–southwest dipolar structure and it is computed based on monthly SST anomalies standardized using the standard deviation for the period 1991–2020 in the South Atlantic Ocean (SAO). The SAD positive phase has a center of positive SST anomalies in the tropical latitudes and a second one of negative anomalies in the subtropics, whereas the negative phase has the opposite pattern. Based on the previous approaches proposed by Morioka et al. (2011) and Nnamchi et al. (2011), Empirical Orthogonal Function (EOF) analysis is applied for each calendar month, and the first EOF mode corresponding to the SAD pattern is then selected. </t>
+  </si>
+  <si>
+    <t>Nogueira et al. (2026)</t>
+  </si>
+  <si>
+    <t>SWSA</t>
+  </si>
+  <si>
+    <t>Southwestern South Atlantic</t>
+  </si>
+  <si>
+    <t>The Southwestern South Atlantic (SWSA) mode is characterized by an intense core of SST anomalies extending from the south–southeastern coast of Brazil toward the eastern Atlantic. The SWSA positive phase has a center of positive SST anomalies in the subtropical latitudes and a second one of negative anomalies in the extratropics, whereas the negative phase has the opposite pattern. In Nogueira et al. (2026), it is observed that in South Atlantic Ocean,  except for the first EOF mode (SAD), the remaining EOFs are not independent. Therefore, they applied a Varimax rotation to redistribute the variance and to obtain a monthly pattern more similar to the SWSA mode previously identified by Kayano et al. (2013). It is important to note that the lack of independence becomes irrelevant after applying the rotation.</t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1036,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}" name="Tabela1" displayName="Tabela1" ref="A1:G26" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G26" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G22">
-    <sortCondition ref="A1:A22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}" name="Tabela1" displayName="Tabela1" ref="A1:G27" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G27" xr:uid="{0504FB2E-E332-4BE4-BA95-9AA42EB46B77}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G23">
+    <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3EAE4E6C-889B-48C6-AAF8-DB3BD35DACB1}" name="Index" dataDxfId="6"/>
@@ -1308,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1328,22 +1337,22 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
@@ -1352,16 +1361,16 @@
     </row>
     <row r="2" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>47</v>
@@ -1370,22 +1379,22 @@
         <v>48</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>35</v>
@@ -1394,22 +1403,22 @@
         <v>36</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>31</v>
@@ -1424,16 +1433,16 @@
     </row>
     <row r="5" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>28</v>
@@ -1448,19 +1457,19 @@
     </row>
     <row r="6" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>40</v>
@@ -1472,19 +1481,19 @@
     </row>
     <row r="7" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
@@ -1496,19 +1505,19 @@
     </row>
     <row r="8" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>8</v>
@@ -1520,19 +1529,19 @@
     </row>
     <row r="9" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>8</v>
@@ -1544,19 +1553,19 @@
     </row>
     <row r="10" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>8</v>
@@ -1568,19 +1577,19 @@
     </row>
     <row r="11" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>39</v>
@@ -1592,16 +1601,16 @@
     </row>
     <row r="12" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>46</v>
@@ -1610,22 +1619,22 @@
         <v>49</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>45</v>
@@ -1634,22 +1643,22 @@
         <v>50</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>44</v>
@@ -1664,73 +1673,73 @@
     </row>
     <row r="15" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -1742,106 +1751,106 @@
         <v>78</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>15</v>
@@ -1854,67 +1863,68 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>113</v>
+        <v>15</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>114</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>120</v>
+        <v>76</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>6</v>
@@ -1925,19 +1935,19 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>124</v>
+        <v>76</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>6</v>
@@ -1947,10 +1957,33 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="6"/>
+      <c r="A27" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1958,13 +1991,13 @@
     <hyperlink ref="F9" r:id="rId2" xr:uid="{245EB88A-FE7C-43E9-9638-22C6D9E40350}"/>
     <hyperlink ref="F10" r:id="rId3" xr:uid="{B9DFECB3-E987-4FF4-9697-4725A45D27B6}"/>
     <hyperlink ref="F7" r:id="rId4" xr:uid="{ECA62230-534D-4F97-8A6C-63B4E3B96DD4}"/>
-    <hyperlink ref="F19" r:id="rId5" location="SOICALC" display="https://www.cpc.ncep.noaa.gov/data/indices/Readme.index.shtml - SOICALC" xr:uid="{B1D8E77E-2473-482E-BCB2-61498215E874}"/>
-    <hyperlink ref="F22" r:id="rId6" xr:uid="{5C08678B-DCCB-4DB1-A396-05DF1D44A233}"/>
-    <hyperlink ref="F21" r:id="rId7" xr:uid="{414AFD97-2A29-45BD-91E9-7FE87FE43269}"/>
-    <hyperlink ref="F16" r:id="rId8" xr:uid="{7D930AD2-BB31-4516-9F29-81BF351BCDBC}"/>
-    <hyperlink ref="F18" r:id="rId9" xr:uid="{C8785809-3965-4F85-A971-059C01941277}"/>
-    <hyperlink ref="F17" r:id="rId10" xr:uid="{9228F806-3134-4A5D-8563-43A5E0031DB2}"/>
-    <hyperlink ref="F20" r:id="rId11" xr:uid="{A3FDF396-DAE3-42F7-87E6-4CAB4933AD41}"/>
+    <hyperlink ref="F20" r:id="rId5" location="SOICALC" display="https://www.cpc.ncep.noaa.gov/data/indices/Readme.index.shtml - SOICALC" xr:uid="{B1D8E77E-2473-482E-BCB2-61498215E874}"/>
+    <hyperlink ref="F23" r:id="rId6" xr:uid="{5C08678B-DCCB-4DB1-A396-05DF1D44A233}"/>
+    <hyperlink ref="F22" r:id="rId7" xr:uid="{414AFD97-2A29-45BD-91E9-7FE87FE43269}"/>
+    <hyperlink ref="F17" r:id="rId8" xr:uid="{7D930AD2-BB31-4516-9F29-81BF351BCDBC}"/>
+    <hyperlink ref="F19" r:id="rId9" xr:uid="{C8785809-3965-4F85-A971-059C01941277}"/>
+    <hyperlink ref="F18" r:id="rId10" xr:uid="{9228F806-3134-4A5D-8563-43A5E0031DB2}"/>
+    <hyperlink ref="F21" r:id="rId11" xr:uid="{A3FDF396-DAE3-42F7-87E6-4CAB4933AD41}"/>
     <hyperlink ref="F5" r:id="rId12" xr:uid="{14120442-89A1-4A75-8BE4-5C765C37105E}"/>
     <hyperlink ref="F4" r:id="rId13" xr:uid="{F20588DE-6804-4152-A357-5A75E889272F}"/>
     <hyperlink ref="F3" r:id="rId14" xr:uid="{0785A3D1-3333-498E-AD13-B78338D847DD}"/>

</xml_diff>